<commit_message>
Stat UI, Card Reward UI
스탯 UI 완성, 카드 보상 선택 UI 진행 중
</commit_message>
<xml_diff>
--- a/Assets/Resources/Data/CardLibrary.xlsx
+++ b/Assets/Resources/Data/CardLibrary.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Unity\capstone-2023-03\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A627F5-FD5C-457F-B19D-3CB8ED8C38D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F0E383-F36C-4402-B7CD-98F42B8480E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{B23A8F8E-BE4C-4BB4-A989-6327509EAC07}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B23A8F8E-BE4C-4BB4-A989-6327509EAC07}"/>
   </bookViews>
   <sheets>
     <sheet name="CardLibrary" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'CardLibrary'!$A$1:$G$23</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'CardLibrary'!$A$1:$G$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>타격</t>
   </si>
@@ -216,6 +216,34 @@
   </si>
   <si>
     <t>attribute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애청자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이번 턴 동안 에너지 2 획득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가속</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>패의 카드 한 장을 이번 전투 동안 코스트 0으로 고정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -300,8 +328,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A54E34B-32F9-4B68-BE81-286E9C397A0E}" name="CardLibrary" displayName="CardLibrary" ref="A1:G23" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G23" xr:uid="{1A54E34B-32F9-4B68-BE81-286E9C397A0E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A54E34B-32F9-4B68-BE81-286E9C397A0E}" name="CardLibrary" displayName="CardLibrary" ref="A1:G26" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G26" xr:uid="{1A54E34B-32F9-4B68-BE81-286E9C397A0E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G23">
     <sortCondition ref="A1:A23"/>
   </sortState>
@@ -615,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6DCCE8-7F42-4F0F-8BED-5D32C8CDC043}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -630,6 +658,7 @@
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
@@ -1159,6 +1188,49 @@
       </c>
       <c r="G23" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Event & GameOver UI
</commit_message>
<xml_diff>
--- a/Assets/Resources/Data/CardLibrary.xlsx
+++ b/Assets/Resources/Data/CardLibrary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Unity\capstone-2023-03\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312D8871-B388-4F14-B571-A3D6D4167E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515E5454-DC6D-4573-96D2-CF30F4FA530E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{B23A8F8E-BE4C-4BB4-A989-6327509EAC07}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'CardLibrary'!$A$1:$G$82</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'CardLibrary'!$A$1:$G$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="181">
   <si>
     <t>타격</t>
   </si>
@@ -651,6 +651,42 @@
   </si>
   <si>
     <t>에너지 2, 힘, 마력 각 1씩 획득</t>
+  </si>
+  <si>
+    <t>레블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카모</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력 15\n무작위 적 1기 2 데미지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력 22\n적 2턴마다 전체 5 x 2 데미지 및 화상 2 부여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력 30\n매 턴마다 에너지 1, 드로우 1 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Partner1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Partner2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Partner3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -737,10 +773,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A54E34B-32F9-4B68-BE81-286E9C397A0E}" name="CardLibrary" displayName="CardLibrary" ref="A1:G82" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G82" xr:uid="{1A54E34B-32F9-4B68-BE81-286E9C397A0E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G82">
-    <sortCondition ref="A1:A82"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A54E34B-32F9-4B68-BE81-286E9C397A0E}" name="CardLibrary" displayName="CardLibrary" ref="A1:G85" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G85" xr:uid="{1A54E34B-32F9-4B68-BE81-286E9C397A0E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G85">
+    <sortCondition ref="A1:A85"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{7CEAE30D-CA72-418A-AAEA-81622FE50B54}" uniqueName="1" name="index" queryTableFieldId="1"/>
@@ -1052,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6DCCE8-7F42-4F0F-8BED-5D32C8CDC043}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1762,45 +1798,45 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>172</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>105</v>
+        <v>178</v>
       </c>
       <c r="G31" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>173</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>105</v>
+        <v>179</v>
       </c>
       <c r="G32" t="s">
         <v>84</v>
@@ -1808,22 +1844,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>174</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="G33" t="s">
         <v>84</v>
@@ -1831,13 +1867,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1846,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="G34" t="s">
         <v>84</v>
@@ -1854,13 +1890,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1869,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="G35" t="s">
         <v>84</v>
@@ -1877,22 +1913,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
         <v>105</v>
-      </c>
-      <c r="B36" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>88</v>
       </c>
       <c r="G36" t="s">
         <v>84</v>
@@ -1900,13 +1936,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1923,13 +1959,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1938,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G38" t="s">
         <v>84</v>
@@ -1946,13 +1982,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1961,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G39" t="s">
         <v>84</v>
@@ -1969,13 +2005,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1984,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G40" t="s">
         <v>84</v>
@@ -1992,13 +2028,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2015,13 +2051,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2038,13 +2074,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2053,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G43" t="s">
         <v>84</v>
@@ -2061,13 +2097,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -2076,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G44" t="s">
         <v>84</v>
@@ -2084,13 +2120,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2099,7 +2135,7 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G45" t="s">
         <v>84</v>
@@ -2107,13 +2143,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2122,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G46" t="s">
         <v>84</v>
@@ -2130,13 +2166,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2145,7 +2181,7 @@
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G47" t="s">
         <v>84</v>
@@ -2153,13 +2189,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2168,7 +2204,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G48" t="s">
         <v>84</v>
@@ -2176,13 +2212,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2191,7 +2227,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G49" t="s">
         <v>84</v>
@@ -2199,13 +2235,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2214,7 +2250,7 @@
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G50" t="s">
         <v>84</v>
@@ -2222,13 +2258,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C51" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2237,7 +2273,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G51" t="s">
         <v>84</v>
@@ -2245,13 +2281,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B52" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2260,7 +2296,7 @@
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="G52" t="s">
         <v>84</v>
@@ -2268,13 +2304,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B53" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2283,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="G53" t="s">
         <v>84</v>
@@ -2291,13 +2327,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C54" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2306,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G54" t="s">
         <v>84</v>
@@ -2314,13 +2350,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A55">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B55" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C55" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2329,7 +2365,7 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="G55" t="s">
         <v>84</v>
@@ -2337,13 +2373,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A56">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C56" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2352,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G56" t="s">
         <v>84</v>
@@ -2360,13 +2396,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B57" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C57" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2375,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G57" t="s">
         <v>84</v>
@@ -2383,13 +2419,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B58" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2398,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G58" t="s">
         <v>84</v>
@@ -2406,13 +2442,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A59">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C59" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2421,7 +2457,7 @@
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G59" t="s">
         <v>84</v>
@@ -2429,13 +2465,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A60">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C60" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2444,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G60" t="s">
         <v>84</v>
@@ -2452,13 +2488,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A61">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B61" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2467,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G61" t="s">
         <v>84</v>
@@ -2475,13 +2511,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A62">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B62" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C62" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2490,7 +2526,7 @@
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G62" t="s">
         <v>84</v>
@@ -2498,13 +2534,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A63">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B63" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C63" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2513,7 +2549,7 @@
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G63" t="s">
         <v>84</v>
@@ -2521,13 +2557,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A64">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -2536,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G64" t="s">
         <v>84</v>
@@ -2544,13 +2580,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A65">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B65" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2559,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G65" t="s">
         <v>84</v>
@@ -2567,13 +2603,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A66">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B66" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C66" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2582,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G66" t="s">
         <v>84</v>
@@ -2590,13 +2626,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A67">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C67" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -2605,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="G67" t="s">
         <v>84</v>
@@ -2613,13 +2649,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A68">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -2628,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="G68" t="s">
         <v>84</v>
@@ -2636,13 +2672,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A69">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C69" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -2651,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="G69" t="s">
         <v>84</v>
@@ -2659,13 +2695,13 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A70">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -2674,7 +2710,7 @@
         <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="G70" t="s">
         <v>84</v>
@@ -2682,13 +2718,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A71">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -2697,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="G71" t="s">
         <v>84</v>
@@ -2705,13 +2741,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A72">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -2720,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G72" t="s">
         <v>84</v>
@@ -2728,13 +2764,13 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A73">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -2743,7 +2779,7 @@
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G73" t="s">
         <v>84</v>
@@ -2751,13 +2787,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A74">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C74" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -2766,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G74" t="s">
         <v>84</v>
@@ -2774,13 +2810,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A75">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C75" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -2789,7 +2825,7 @@
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G75" t="s">
         <v>84</v>
@@ -2797,13 +2833,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A76">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C76" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -2812,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G76" t="s">
         <v>84</v>
@@ -2820,13 +2856,13 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A77">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C77" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2835,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G77" t="s">
         <v>84</v>
@@ -2843,13 +2879,13 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A78">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B78" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C78" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -2858,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G78" t="s">
         <v>84</v>
@@ -2866,22 +2902,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A79">
-        <v>1000</v>
+        <v>145</v>
       </c>
       <c r="B79" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C79" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="G79" t="s">
         <v>84</v>
@@ -2889,22 +2925,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A80">
-        <v>1001</v>
+        <v>146</v>
       </c>
       <c r="B80" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C80" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
       <c r="E80">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="G80" t="s">
         <v>84</v>
@@ -2912,22 +2948,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A81">
-        <v>1002</v>
+        <v>147</v>
       </c>
       <c r="B81" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>66</v>
+        <v>151</v>
       </c>
       <c r="D81">
         <v>0</v>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="G81" t="s">
         <v>84</v>
@@ -2935,10 +2971,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A82">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="B82" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="C82" t="s">
         <v>66</v>
@@ -2950,9 +2986,78 @@
         <v>2</v>
       </c>
       <c r="F82" t="s">
+        <v>99</v>
+      </c>
+      <c r="G82" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A83">
+        <v>1001</v>
+      </c>
+      <c r="B83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83" t="s">
+        <v>100</v>
+      </c>
+      <c r="G83" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A84">
+        <v>1002</v>
+      </c>
+      <c r="B84" t="s">
+        <v>67</v>
+      </c>
+      <c r="C84" t="s">
+        <v>66</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s">
+        <v>102</v>
+      </c>
+      <c r="G84" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A85">
+        <v>1003</v>
+      </c>
+      <c r="B85" t="s">
+        <v>68</v>
+      </c>
+      <c r="C85" t="s">
+        <v>66</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85" t="s">
         <v>104</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G85" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>